<commit_message>
Wilschers abwesenheit eingetragen (und Sunnys)
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -65,7 +65,7 @@
     <t>Santner</t>
   </si>
   <si>
-    <t>Wilscher krank</t>
+    <t>Wilscher krank!</t>
   </si>
   <si>
     <r>
@@ -77,7 +77,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Sunny krank</t>
+      <t>Sunny krank!</t>
     </r>
     <r>
       <rPr>
@@ -87,7 +87,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>;Menü verbessert</t>
+      <t>; Menü verbessert</t>
     </r>
   </si>
 </sst>
@@ -195,13 +195,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7">
@@ -565,56 +565,56 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="7">
         <v>42810</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="7">
         <v>42811</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="7">
         <v>42814</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="7">
         <v>42815</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="7">
         <v>42816</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="7">
         <v>42817</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="7">
         <v>42818</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="7">
         <v>42821</v>
       </c>
@@ -623,7 +623,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="7">
         <v>42822</v>
       </c>
@@ -632,7 +632,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="7">
         <v>42823</v>
       </c>
@@ -641,7 +641,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="7">
         <v>42824</v>
       </c>
@@ -671,18 +671,18 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="7">
         <v>42825</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="7">
         <v>42844</v>
       </c>
@@ -691,37 +691,37 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="7">
         <v>42845</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="7">
         <v>42846</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="7">
         <v>42849</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="7">
         <v>42850</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="7">
         <v>42851</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="7">
         <v>42852</v>
       </c>

</xml_diff>

<commit_message>
Gonna Push fast (Sprintziel eingetragen)
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Sprint</t>
   </si>
@@ -89,6 +89,9 @@
       </rPr>
       <t>; Menü verbessert</t>
     </r>
+  </si>
+  <si>
+    <t>Fertigstellung der Klassen, des Menüs, der Spielerstellung und der Spieleranlegung</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -201,6 +204,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,14 +530,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="6" max="6" width="90.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -668,6 +674,9 @@
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Sprints document, added Sprint2_Review
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\AndroidStudioProjects\Soccer_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Elias\StudioProjects\Soccer_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -97,10 +97,10 @@
     <t>Keinen Fortschritt gemacht</t>
   </si>
   <si>
-    <t>Kein Fortschritt</t>
-  </si>
-  <si>
     <t>Erfolgreich branch auf sprint2 umgestellt</t>
+  </si>
+  <si>
+    <t>Add Player implementiert</t>
   </si>
 </sst>
 </file>
@@ -539,19 +539,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="6" max="6" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
@@ -579,56 +579,56 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="7">
         <v>42810</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="7">
         <v>42811</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="7">
         <v>42814</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="7">
         <v>42815</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="7">
         <v>42816</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="7">
         <v>42817</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="7">
         <v>42818</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="7">
         <v>42821</v>
@@ -637,7 +637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="7">
         <v>42822</v>
@@ -646,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="7">
         <v>42823</v>
@@ -655,7 +655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="7">
         <v>42824</v>
@@ -664,11 +664,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
@@ -688,7 +688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
@@ -699,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="7">
         <v>42844</v>
@@ -708,7 +708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="7">
         <v>42845</v>
@@ -717,37 +717,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="7">
         <v>42846</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="7">
         <v>42849</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="7">
         <v>42850</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="7">
         <v>42851</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="7">
         <v>42852</v>

</xml_diff>

<commit_message>
Klassen in entsprechende Packages eingeteilt, DailyScrum festgehalten
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\AndroidStudioProjects\Soccer_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Documents\AndroidProjects\Soccer_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Sprint</t>
   </si>
@@ -146,6 +146,12 @@
       <t>Besprechung für Spiel anlegen/bearbeiten Konzept, Scrumboard für Sprint geändert</t>
     </r>
   </si>
+  <si>
+    <t>Frei!</t>
+  </si>
+  <si>
+    <t>Besprechung Menü und SpielerstellungsGUIs</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd\ \-\ dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +216,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -243,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,6 +282,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -591,7 +606,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,11 +857,17 @@
       <c r="B27" s="6">
         <v>42856</v>
       </c>
+      <c r="C27" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="6">
         <v>42857</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Sprints-document and Storymap
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Sprint</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Spieler für Spiel auswählen fertig</t>
   </si>
   <si>
-    <t xml:space="preserve">Sunny krank!;  </t>
-  </si>
-  <si>
     <t>Player bearbeiten/löschen fertig; Zusammenführung Spiel erstellen</t>
   </si>
   <si>
@@ -204,10 +201,30 @@
     <t>4. Sprint</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Spiel bearbeiten/löschen, Statistiken, Rollen implementieren, Für Präsentation vorbereiten</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sunny krank!;  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Planung neuer Sprint</t>
+    </r>
+  </si>
+  <si>
+    <t>Zuweisung der Aufgaben</t>
+  </si>
+  <si>
+    <t>Generelle Besprechung und Bugfixes, Rollen implementiert, Layout verbessert</t>
+  </si>
+  <si>
+    <t>Lagebesprechung, Gameliste anzeigen</t>
   </si>
 </sst>
 </file>
@@ -316,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -345,6 +362,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -667,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,7 +886,7 @@
         <v>42850</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -886,7 +904,7 @@
         <v>42852</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -944,7 +962,7 @@
         <v>42858</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,7 +989,7 @@
         <v>42863</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -980,7 +998,7 @@
         <v>42864</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -989,7 +1007,7 @@
         <v>42865</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -998,7 +1016,7 @@
         <v>42866</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1012,21 +1030,24 @@
         <v>4</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="6">
         <v>42867</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1034,12 +1055,17 @@
       <c r="B39" s="6">
         <v>42870</v>
       </c>
-      <c r="C39" s="8"/>
+      <c r="C39" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
       <c r="B40" s="6">
         <v>42871</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
teamzuteilung swipe, animation fertiggestellt muss nur noch auf Player angepasst werden Shuffle, und die einbindung in spiel erstellen
</commit_message>
<xml_diff>
--- a/documents/Sprints.xlsx
+++ b/documents/Sprints.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Elias\StudioProjects\Soccer_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Documents\AndroidProjects\Soccer_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Sprint</t>
   </si>
@@ -225,6 +225,24 @@
   </si>
   <si>
     <t>Lagebesprechung, Gameliste anzeigen</t>
+  </si>
+  <si>
+    <t>Vorbereitung für Präsentation</t>
+  </si>
+  <si>
+    <t>Layout für Tablets erstellt</t>
+  </si>
+  <si>
+    <t>Kleinere Bugfixes</t>
+  </si>
+  <si>
+    <t>Besprechung bzgl. Präsentration</t>
+  </si>
+  <si>
+    <t>Letzte Bugfixes für Präsentation</t>
+  </si>
+  <si>
+    <t>Besprechung des neuen Sprints mithilfe der neu gewonnen Ideen der Präsentationen</t>
   </si>
 </sst>
 </file>
@@ -356,13 +374,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -683,21 +701,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="113" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -717,65 +735,65 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6">
         <v>42809</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
       <c r="B3" s="6">
         <v>42810</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="6">
         <v>42811</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="6">
         <v>42814</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
       <c r="B6" s="6">
         <v>42815</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="B7" s="6">
         <v>42816</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="6">
         <v>42817</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="6">
         <v>42818</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="6">
         <v>42821</v>
       </c>
@@ -783,8 +801,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="6">
         <v>42822</v>
       </c>
@@ -792,8 +810,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="6">
         <v>42823</v>
       </c>
@@ -801,8 +819,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
       <c r="B13" s="6">
         <v>42824</v>
       </c>
@@ -810,10 +828,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
@@ -833,8 +851,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6">
@@ -844,8 +862,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
       <c r="B17" s="6">
         <v>42844</v>
       </c>
@@ -853,8 +871,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
       <c r="B18" s="6">
         <v>42845</v>
       </c>
@@ -862,8 +880,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
       <c r="B19" s="6">
         <v>42846</v>
       </c>
@@ -871,8 +889,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" s="6">
         <v>42849</v>
       </c>
@@ -880,8 +898,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
       <c r="B21" s="6">
         <v>42850</v>
       </c>
@@ -889,8 +907,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
       <c r="B22" s="6">
         <v>42851</v>
       </c>
@@ -898,8 +916,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
       <c r="B23" s="6">
         <v>42852</v>
       </c>
@@ -907,7 +925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>0</v>
       </c>
@@ -927,8 +945,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="6">
@@ -938,8 +956,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="6">
         <v>42856</v>
       </c>
@@ -947,8 +965,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
       <c r="B28" s="6">
         <v>42857</v>
       </c>
@@ -956,8 +974,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
       <c r="B29" s="6">
         <v>42858</v>
       </c>
@@ -965,8 +983,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="6">
         <v>42859</v>
       </c>
@@ -974,8 +992,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="6">
         <v>42860</v>
       </c>
@@ -983,8 +1001,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="6">
         <v>42863</v>
       </c>
@@ -992,8 +1010,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="6">
         <v>42864</v>
       </c>
@@ -1001,8 +1019,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
       <c r="B34" s="6">
         <v>42865</v>
       </c>
@@ -1010,8 +1028,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
       <c r="B35" s="6">
         <v>42866</v>
       </c>
@@ -1019,7 +1037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
@@ -1039,8 +1057,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
+    <row r="38" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="6">
@@ -1050,17 +1068,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
       <c r="B39" s="6">
         <v>42870</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
       <c r="B40" s="6">
         <v>42871</v>
       </c>
@@ -1068,48 +1086,71 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
       <c r="B41" s="6">
         <v>42872</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
       <c r="B42" s="6">
         <v>42873</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
       <c r="B43" s="6">
         <v>42874</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
       <c r="B44" s="6">
         <v>42877</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
+      <c r="C44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
       <c r="B45" s="6">
         <v>42878</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
       <c r="B46" s="6">
         <v>42879</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
       <c r="B47" s="6">
         <v>42880</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>